<commit_message>
Exploring this from past...
Weeks later, hopefully didn't break anything...

It seems to be the most recent attempt with good formulas, and reads folder from worksheet, blah, blah, blah...
</commit_message>
<xml_diff>
--- a/tracking.xlsx
+++ b/tracking.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t-ste\Documents\GitHub\2023-spring\adv-fe-tuth\tca-roll-for-it\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t-ste\Documents\GitHub\2023-fall\adv-fe\tca-roll-for-it\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81297F65-4AB8-42EE-BB0F-DB8AA02E40E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8164BF-28A1-4A02-9164-519014AE6B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="18426" windowHeight="11626" activeTab="2" xr2:uid="{20210E21-2C27-4F76-B1A2-68AB3FCAC5C6}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="33" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -270,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -278,7 +278,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -1783,7 +1782,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D86176C2-F5C2-4A83-B9B1-B801288A038D}" name="PivotTable1" cacheId="33" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Work Buckets" colHeaderCaption="Dates">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D86176C2-F5C2-4A83-B9B1-B801288A038D}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Work Buckets" colHeaderCaption="Dates">
   <location ref="A1:I24" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" defaultSubtotal="0">
@@ -2346,7 +2345,7 @@
       </c>
       <c r="B2" t="str" cm="1">
         <f t="array" aca="1" ref="B2" ca="1">LEFT(CELL("filename",A1),FIND("[",CELL("filename",A1))-1)</f>
-        <v>C:\Users\t-ste\Documents\GitHub\2023-spring\adv-fe-tuth\tca-roll-for-it\</v>
+        <v>C:\Users\t-ste\Documents\GitHub\2023-fall\adv-fe\tca-roll-for-it\</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.5">
@@ -2371,7 +2370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEB0F96B-5C21-4424-B26A-F6EAEBE0362D}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -2447,18 +2446,13 @@
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5">
+      <c r="D4">
         <v>-1</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5">
+      <c r="I4">
         <v>0</v>
       </c>
     </row>
@@ -2466,302 +2460,207 @@
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6">
         <v>0</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5">
+      <c r="I6">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5">
+      <c r="H8">
         <v>10</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9">
         <v>0.5</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9">
         <v>-0.5</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5">
+      <c r="I9">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5">
+      <c r="G10">
         <v>2</v>
       </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5">
+      <c r="I10">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11">
         <v>0.5</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5">
+      <c r="D11">
         <v>-0.5</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5">
+      <c r="I11">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12">
         <v>0.5</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5">
+      <c r="D12">
         <v>-0.5</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5">
+      <c r="I12">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13">
         <v>0</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5">
+      <c r="I13">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14">
         <v>0.5</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14">
         <v>-0.5</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5">
+      <c r="I14">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15">
         <v>2</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15">
         <v>-2</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5">
+      <c r="I15">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5">
+      <c r="E16">
         <v>0</v>
       </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5">
+      <c r="I16">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17">
         <v>0.25</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5">
+      <c r="D17">
         <v>-0.25</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5">
+      <c r="I17">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18">
         <v>1</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18">
         <v>-1</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5">
+      <c r="I18">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19">
         <v>1.5</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5">
+      <c r="D19">
         <v>-1.5</v>
       </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5">
+      <c r="I19">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20">
         <v>7</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20">
         <v>-6.5</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20">
         <v>-0.5</v>
       </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5">
+      <c r="I20">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21">
         <v>0.5</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21">
         <v>-0.5</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5">
+      <c r="I21">
         <v>0</v>
       </c>
     </row>
@@ -2769,18 +2668,13 @@
       <c r="A22" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22">
         <v>2.75</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5">
+      <c r="D22">
         <v>-2.75</v>
       </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5">
+      <c r="I22">
         <v>0</v>
       </c>
     </row>
@@ -2788,22 +2682,19 @@
       <c r="A23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23">
         <v>5.25</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23">
         <v>0</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23">
         <v>-4.75</v>
       </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5">
+      <c r="F23">
         <v>-0.5</v>
       </c>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5">
+      <c r="I23">
         <v>0</v>
       </c>
     </row>
@@ -2811,28 +2702,28 @@
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24">
         <v>23.25</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24">
         <v>-11</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24">
         <v>-11.75</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24">
         <v>0</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24">
         <v>-0.5</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24">
         <v>2</v>
       </c>
-      <c r="H24" s="5">
+      <c r="H24">
         <v>10</v>
       </c>
-      <c r="I24" s="5">
+      <c r="I24">
         <v>12</v>
       </c>
     </row>
@@ -2846,7 +2737,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection sqref="A1:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>